<commit_message>
Finished beautiful_soup.py, ready to be seeded.
</commit_message>
<xml_diff>
--- a/seed_data/char_data.xlsx
+++ b/seed_data/char_data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="4960" yWindow="1860" windowWidth="12780" windowHeight="15880" tabRatio="500"/>
+    <workbookView xWindow="1600" yWindow="1820" windowWidth="12780" windowHeight="15880" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="31">
   <si>
     <t>Characteristic</t>
   </si>
@@ -127,7 +127,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -138,6 +138,11 @@
     <font>
       <sz val="14"/>
       <color theme="1"/>
+      <name val="Menlo"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FFD6D6D6"/>
       <name val="Menlo"/>
     </font>
   </fonts>
@@ -161,10 +166,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -180,8 +186,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:A15" totalsRowShown="0">
-  <autoFilter ref="A1:A15"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:A16" totalsRowShown="0">
+  <autoFilter ref="A1:A16"/>
   <tableColumns count="1">
     <tableColumn id="1" name="Characteristic"/>
   </tableColumns>
@@ -455,10 +461,10 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <tabColor theme="7"/>
   </sheetPr>
-  <dimension ref="A1:A15"/>
+  <dimension ref="A1:A18"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -518,28 +524,36 @@
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
         <v>11</v>
       </c>
+    </row>
+    <row r="18" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A18" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>